<commit_message>
feat: some more updates
</commit_message>
<xml_diff>
--- a/Test Outcomes.xlsx
+++ b/Test Outcomes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamie/Documents/programming/gpt-promises-api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386487AF-ACD8-ED42-889B-11BDF78FD82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7490540-50D0-5643-ADB1-4277C8576F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="25100" xr2:uid="{37D27B90-CC1A-AD4C-BCF7-9C690B2C4802}"/>
   </bookViews>
@@ -501,7 +501,7 @@
   <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D3" sqref="D3:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>